<commit_message>
Revamped and Added New Examples
Aspose.Cells for .NET
</commit_message>
<xml_diff>
--- a/Examples/Data/Articles/ManagingWorkbooksWorksheets/CopyMoveWorksheets/FirstWorkbook.xlsx
+++ b/Examples/Data/Articles/ManagingWorkbooksWorksheets/CopyMoveWorksheets/FirstWorkbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Copy" sheetId="1" r:id="rId1"/>
@@ -16,38 +16,105 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>City</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="30">
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Salesperson</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>OrderID</t>
+  </si>
+  <si>
+    <t>Order Amount</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Suyama</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Leverling</t>
+  </si>
+  <si>
+    <t>Peacock</t>
+  </si>
+  <si>
+    <t>Buchanan</t>
+  </si>
+  <si>
+    <t>Dodsworth</t>
+  </si>
+  <si>
+    <t>Davolio</t>
+  </si>
+  <si>
+    <t>Callahan</t>
+  </si>
+  <si>
+    <t>Fuller</t>
+  </si>
+  <si>
+    <t>cl</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>Beverage</t>
+  </si>
+  <si>
+    <t>Chai</t>
+  </si>
+  <si>
+    <t>Chang</t>
+  </si>
+  <si>
+    <t>Chartreuse</t>
   </si>
   <si>
     <t>John</t>
   </si>
   <si>
-    <t>john@doe.com</t>
-  </si>
-  <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>Salary</t>
-  </si>
-  <si>
-    <t>John Doe</t>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Ipoh</t>
+  </si>
+  <si>
+    <t>Qtr 1</t>
+  </si>
+  <si>
+    <t>Qtr 2</t>
+  </si>
+  <si>
+    <t>Qtr 3</t>
+  </si>
+  <si>
+    <t>Qtr 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -58,9 +125,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,17 +150,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -393,163 +460,931 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <v>37818</v>
+      </c>
+      <c r="D2">
+        <v>10248</v>
+      </c>
+      <c r="E2" s="3">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>37812</v>
+      </c>
+      <c r="D3">
+        <v>10249</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1863.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>37814</v>
+      </c>
+      <c r="D4">
+        <v>10250</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1552.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>37817</v>
+      </c>
+      <c r="D5">
+        <v>10251</v>
+      </c>
+      <c r="E5" s="4">
+        <v>654.05999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>37813</v>
+      </c>
+      <c r="D6">
+        <v>10252</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3597.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>37818</v>
+      </c>
+      <c r="D7">
+        <v>10253</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1444.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
+        <v>37825</v>
+      </c>
+      <c r="D8">
+        <v>10254</v>
+      </c>
+      <c r="E8" s="3">
+        <v>556.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>37817</v>
+      </c>
+      <c r="D9">
+        <v>10255</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2493.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>37819</v>
+      </c>
+      <c r="D10">
+        <v>10256</v>
+      </c>
+      <c r="E10" s="3">
+        <v>517.79999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2">
+        <v>37824</v>
+      </c>
+      <c r="D11">
+        <v>10257</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1119.9000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2">
+        <v>37825</v>
+      </c>
+      <c r="D12">
+        <v>10258</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1614.88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2">
+        <v>37827</v>
+      </c>
+      <c r="D13">
+        <v>10259</v>
+      </c>
+      <c r="E13" s="3">
+        <v>100.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2">
+        <v>37831</v>
+      </c>
+      <c r="D14">
+        <v>10260</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1504.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2">
+        <v>37832</v>
+      </c>
+      <c r="D15">
+        <v>10261</v>
+      </c>
+      <c r="E15" s="3">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2">
+        <v>37827</v>
+      </c>
+      <c r="D16">
+        <v>10262</v>
+      </c>
+      <c r="E16" s="3">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2">
+        <v>37833</v>
+      </c>
+      <c r="D17">
+        <v>10263</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1873.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2">
+        <v>37856</v>
+      </c>
+      <c r="D18">
+        <v>10264</v>
+      </c>
+      <c r="E18" s="3">
+        <v>695.62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2">
+        <v>37845</v>
+      </c>
+      <c r="D19">
+        <v>10265</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2">
+        <v>37833</v>
+      </c>
+      <c r="D20">
+        <v>10266</v>
+      </c>
+      <c r="E20" s="3">
+        <v>346.56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="2">
+        <v>37839</v>
+      </c>
+      <c r="D21">
+        <v>10267</v>
+      </c>
+      <c r="E21" s="3">
+        <v>3536.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2">
+        <v>37835</v>
+      </c>
+      <c r="D22">
+        <v>10268</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1101.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="2">
+        <v>37863</v>
+      </c>
+      <c r="D23">
+        <v>10269</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2">
+        <v>37842</v>
+      </c>
+      <c r="D24">
+        <v>10270</v>
+      </c>
+      <c r="E24" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2">
+        <v>37839</v>
+      </c>
+      <c r="D25">
+        <v>10271</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="2">
+        <v>37835</v>
+      </c>
+      <c r="D26">
+        <v>10272</v>
+      </c>
+      <c r="E26" s="3">
+        <v>2037.28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="2">
+        <v>37836</v>
+      </c>
+      <c r="D27">
+        <v>10273</v>
+      </c>
+      <c r="E27" s="3">
+        <v>538.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="2">
+        <v>37842</v>
+      </c>
+      <c r="D28">
+        <v>10274</v>
+      </c>
+      <c r="E28" s="3">
+        <v>291.83999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="2">
+        <v>37845</v>
+      </c>
+      <c r="D29">
+        <v>10275</v>
+      </c>
+      <c r="E29" s="3">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2">
+        <v>37849</v>
+      </c>
+      <c r="D30">
+        <v>10276</v>
+      </c>
+      <c r="E30" s="3">
+        <v>642.20000000000005</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3:B7" r:id="rId2" display="john@doe.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1863.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1552.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4">
+        <v>654.05999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5000</v>
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3597.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1444.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3">
+        <v>556.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2493.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3">
+        <v>517.79999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1119.9000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1614.88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="3">
+        <v>100.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1504.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="3">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1873.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="3">
+        <v>695.62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="3">
+        <v>346.56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="3">
+        <v>3536.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1101.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="3">
+        <v>2037.28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="3">
+        <v>538.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="3">
+        <v>291.83999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="3">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="3">
+        <v>642.20000000000005</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>